<commit_message>
add invalid cases in add user class enhancement in edit page
</commit_message>
<xml_diff>
--- a/src/test/resources/testDataExcelFiles/UsersTD.xlsx
+++ b/src/test/resources/testDataExcelFiles/UsersTD.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8F3BAB-87EE-4F6D-810F-F616E258F90F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4678B22-F557-43A0-9183-2A561D773C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ListRoles" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="72">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -212,13 +212,40 @@
   </si>
   <si>
     <t>Verify edit User Password Settings [mustChangePassword Flag]</t>
+  </si>
+  <si>
+    <t>error type</t>
+  </si>
+  <si>
+    <t>notification</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>Invalid Email</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Invalid Email#required#Please Select User Role</t>
+  </si>
+  <si>
+    <t>Please Select User Role</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>Manage Users</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +265,33 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -302,10 +356,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -313,48 +368,48 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{599A2DD6-9A63-48B3-AC49-370526ACCD11}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -638,7 +693,7 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
@@ -647,7 +702,7 @@
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,7 +719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -677,7 +732,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -690,7 +745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -709,285 +764,442 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF868B8-2750-41BC-92AB-F9E96DC68C16}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:J1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6:L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="67.88671875" style="5" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.44140625" customWidth="1"/>
+    <col min="12" max="12" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:12" ht="18">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="18">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="14" t="s">
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="11">
-        <v>0</v>
-      </c>
-      <c r="J2" s="11">
-        <v>0</v>
-      </c>
-      <c r="K2" s="11" t="s">
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row r="7" spans="1:12" ht="18">
+      <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="F7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I7" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J7" s="2">
         <v>1</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K7" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+    <row r="8" spans="1:12" ht="18">
+      <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="14" t="s">
+      <c r="F8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="11">
-        <v>0</v>
-      </c>
-      <c r="J4" s="11">
-        <v>0</v>
-      </c>
-      <c r="K4" s="11" t="s">
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+    <row r="9" spans="1:12" ht="18">
+      <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="14" t="s">
+      <c r="F9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="11">
-        <v>0</v>
-      </c>
-      <c r="J5" s="11">
-        <v>0</v>
-      </c>
-      <c r="K5" s="11" t="s">
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+    <row r="10" spans="1:12" ht="18">
+      <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="14" t="s">
+      <c r="F10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="11">
-        <v>0</v>
-      </c>
-      <c r="J6" s="11">
-        <v>0</v>
-      </c>
-      <c r="K6" s="11" t="s">
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+    <row r="11" spans="1:12" ht="18">
+      <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="14" t="s">
+      <c r="F11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I11" s="2">
         <v>1</v>
       </c>
-      <c r="J7" s="11">
-        <v>0</v>
-      </c>
-      <c r="K7" s="11" t="s">
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+    <row r="12" spans="1:12" ht="18">
+      <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="14" t="s">
+      <c r="F12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="11">
-        <v>0</v>
-      </c>
-      <c r="J8" s="11">
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
         <v>1</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K12" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1005,7 +1217,7 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
@@ -1015,107 +1227,107 @@
     <col min="6" max="6" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="15" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="19"/>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" ht="28.8">
+      <c r="A4" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:6" ht="28.8">
+      <c r="A5" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:6" ht="28.8">
+      <c r="A6" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="15" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1125,125 +1337,163 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472D54A-51ED-4B16-A05B-B0F68AEDD45E}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="52.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="7" max="7" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20" t="s">
+      <c r="I1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
+      <c r="I2" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18">
+      <c r="A3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="20"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20" t="s">
+      <c r="I3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="I4" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
         <v>60</v>
       </c>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>61</v>
+      <c r="I5" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>60</v>
+      <c r="H6" s="2"/>
+      <c r="I6" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change env url change user credentials
</commit_message>
<xml_diff>
--- a/src/test/resources/testDataExcelFiles/UsersTD.xlsx
+++ b/src/test/resources/testDataExcelFiles/UsersTD.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4678B22-F557-43A0-9183-2A561D773C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51B8A93-1824-4BA6-958E-028560A33741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="81">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -239,6 +239,33 @@
   </si>
   <si>
     <t>Manage Users</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>nayra</t>
+  </si>
+  <si>
+    <t>Verify add new user without Role</t>
+  </si>
+  <si>
+    <t>nahla</t>
+  </si>
+  <si>
+    <t>Verify add new user without phone</t>
+  </si>
+  <si>
+    <t>nero</t>
+  </si>
+  <si>
+    <t>Verify add new user without mail and role</t>
+  </si>
+  <si>
+    <t>mostafa</t>
+  </si>
+  <si>
+    <t>011</t>
   </si>
 </sst>
 </file>
@@ -764,10 +791,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF868B8-2750-41BC-92AB-F9E96DC68C16}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -775,15 +802,16 @@
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.88671875" style="5" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.44140625" customWidth="1"/>
-    <col min="12" max="12" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.44140625" customWidth="1"/>
+    <col min="13" max="13" width="39.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -794,166 +822,181 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18">
+    <row r="2" spans="1:13" ht="18">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
       <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="L2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="18">
+    <row r="3" spans="1:13" ht="18">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="F3" s="10"/>
       <c r="G3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
       <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
         <v>1</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="L3" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="18">
+    <row r="4" spans="1:13" ht="18">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="D4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
       <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
         <v>1</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="L4" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18">
+    <row r="5" spans="1:13" ht="18">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="G5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
       <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
         <v>1</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="L5" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="18">
+    <row r="6" spans="1:13" ht="18">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -962,32 +1005,35 @@
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="12" t="s">
+      <c r="G6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
       <c r="J6" s="2">
         <v>0</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="18">
+    <row r="7" spans="1:13" ht="18">
       <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
@@ -996,34 +1042,37 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="G7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1</v>
       </c>
       <c r="J7" s="2">
         <v>1</v>
       </c>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="18">
+    <row r="8" spans="1:13" ht="18">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -1032,34 +1081,37 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="G8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="2">
-        <v>0</v>
-      </c>
       <c r="J8" s="2">
         <v>0</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18">
+    <row r="9" spans="1:13" ht="18">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -1068,34 +1120,37 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="G9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="2">
-        <v>0</v>
-      </c>
       <c r="J9" s="2">
         <v>0</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="18">
+    <row r="10" spans="1:13" ht="18">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -1104,34 +1159,37 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="G10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
       <c r="J10" s="2">
         <v>0</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="18">
+    <row r="11" spans="1:13" ht="18">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -1140,34 +1198,37 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>36</v>
+      <c r="F11" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>1</v>
       </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="18">
+    <row r="12" spans="1:13" ht="18">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -1176,30 +1237,33 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="G12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="2">
-        <v>0</v>
-      </c>
       <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
         <v>1</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="L12" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1337,10 +1401,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F472D54A-51ED-4B16-A05B-B0F68AEDD45E}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1391,16 +1455,16 @@
         <v>59</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="20" t="s">
         <v>70</v>
       </c>
@@ -1408,44 +1472,44 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="20" t="s">
         <v>70</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="18">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="18" t="s">
         <v>70</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -1454,18 +1518,18 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="20" t="s">
         <v>70</v>
@@ -1476,23 +1540,45 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>60</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="20" t="s">
         <v>70</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>71</v>
       </c>
     </row>

</xml_diff>